<commit_message>
Add code saving results
</commit_message>
<xml_diff>
--- a/animals/annelids/annelid_biomass_data.xlsx
+++ b/animals/annelids/annelid_biomass_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Fierer" sheetId="1" state="visible" r:id="rId2"/>
@@ -181,7 +181,7 @@
     <t xml:space="preserve">http://dx.doi.org/10.1007/s003740050469</t>
   </si>
   <si>
-    <t xml:space="preserve">Taken from Table 5.3 in Biogeochemistry by </t>
+    <t xml:space="preserve">Taken from Table 5.3 in Biogeochemistry: An analysis of Global Change by Schlesinger &amp; Bernhardt.</t>
   </si>
   <si>
     <t xml:space="preserve">Area [m^2]</t>
@@ -206,6 +206,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -226,6 +227,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -316,10 +318,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.0510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.75"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.0510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.5612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.5612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -558,13 +560,13 @@
   </sheetPr>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="2" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="2" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -592,6 +594,7 @@
       <c r="H1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="I1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
@@ -615,6 +618,8 @@
       <c r="G2" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
@@ -635,6 +640,9 @@
       <c r="F3" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
@@ -655,6 +663,9 @@
       <c r="F4" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="G4" s="0"/>
+      <c r="H4" s="0"/>
+      <c r="I4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
@@ -675,6 +686,9 @@
       <c r="F5" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="G5" s="0"/>
+      <c r="H5" s="0"/>
+      <c r="I5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
@@ -695,6 +709,9 @@
       <c r="F6" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="G6" s="0"/>
+      <c r="H6" s="0"/>
+      <c r="I6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
@@ -721,6 +738,7 @@
       <c r="H7" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="I7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
@@ -747,6 +765,7 @@
       <c r="H8" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="I8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
@@ -822,6 +841,7 @@
       <c r="G11" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="I11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="n">
@@ -950,7 +970,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -965,14 +985,14 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.9387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.6224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1089,7 +1109,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>